<commit_message>
workaround for people with no phone or email
</commit_message>
<xml_diff>
--- a/Test Parliament.xlsx
+++ b/Test Parliament.xlsx
@@ -233,6 +233,24 @@
   </x:si>
   <x:si>
     <x:t>gary.anand@parl.gc.ca</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Anderson, Scott</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ourcommons.ca/Members/en/scott-anderson(89259)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vernon—Lake Country—Monashee</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ourcommons.ca/Members/en/constituencies/vernon-lake-country-monashee(1280)</x:t>
+  </x:si>
+  <x:si>
+    <x:t/>
+  </x:si>
+  <x:si>
+    <x:t>scott.anderson@parl.gc.ca</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -875,6 +893,32 @@
         <x:v>72</x:v>
       </x:c>
     </x:row>
+    <x:row r="12" spans="1:8">
+      <x:c r="A12" s="0" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E12" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="F12" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="G12" s="0" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="H12" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
changing telephone element so it's better at determining if there is one or not
</commit_message>
<xml_diff>
--- a/Test Parliament.xlsx
+++ b/Test Parliament.xlsx
@@ -40,109 +40,106 @@
     <x:t>Email</x:t>
   </x:si>
   <x:si>
-    <x:t>Aboultaif, Ziad</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ourcommons.ca/Members/en/ziad-aboultaif(89156)</x:t>
+    <x:t>https://www.ourcommons.ca/Members/en/carol-anstey(109872)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Long Range Mountains</x:t>
   </x:si>
   <x:si>
     <x:t>Conservative</x:t>
   </x:si>
   <x:si>
-    <x:t>Edmonton Manning</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ourcommons.ca/Members/en/constituencies/edmonton-manning(1220)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Alberta</x:t>
-  </x:si>
-  <x:si>
-    <x:t>780-822-1540</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ziad.aboultaif@parl.gc.ca</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Acan, Sima</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ourcommons.ca/Members/en/sima-acan(123092)</x:t>
+    <x:t>https://www.ourcommons.ca/Members/en/constituencies/long-range-mountains(947)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Newfoundland and Labrador</x:t>
+  </x:si>
+  <x:si>
+    <x:t>709-637-4655</x:t>
+  </x:si>
+  <x:si>
+    <x:t>carol.anstey@parl.gc.ca</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Arnold, Mel</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ourcommons.ca/Members/en/mel-arnold(89294)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kamloops—Shuswap—Central Rockies</x:t>
   </x:si>
   <x:si>
     <x:t>Liberal</x:t>
   </x:si>
   <x:si>
-    <x:t>Oakville West</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ourcommons.ca/Members/en/constituencies/oakville-west(1128)</x:t>
+    <x:t>https://www.ourcommons.ca/Members/en/constituencies/kamloops-shuswap-central-rockies(1253)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>778-283-9700</x:t>
   </x:si>
   <x:si>
     <x:t>Ontario</x:t>
   </x:si>
   <x:si>
-    <x:t>905-847-4907</x:t>
-  </x:si>
-  <x:si>
-    <x:t>sima.acan@parl.gc.ca</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Aitchison, Scott</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ourcommons.ca/Members/en/scott-aitchison(105340)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Parry Sound—Muskoka</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ourcommons.ca/Members/en/constituencies/parry-sound-muskoka(1136)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>705-789-4640</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Scott.Aitchison@parl.gc.ca</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Al Soud, Fares</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ourcommons.ca/Members/en/fares-al-soud(123033)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mississauga Centre</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ourcommons.ca/Members/en/constituencies/mississauga-centre(1113)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>905-848-7855</x:t>
-  </x:si>
-  <x:si>
-    <x:t>fares.alsoud@parl.gc.ca</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Albas, Dan</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ourcommons.ca/Members/en/dan-albas(72029)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Okanagan Lake West—South Kelowna</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ourcommons.ca/Members/en/constituencies/okanagan-lake-west-south-kelowna(1262)</x:t>
+    <x:t>mel.arnold@parl.gc.ca</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Au, Chak</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ourcommons.ca/Members/en/chak-au(123608)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Richmond Centre—Marpole</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ourcommons.ca/Members/en/constituencies/richmond-centre-marpole(1266)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>450-964-4919</x:t>
+  </x:si>
+  <x:si>
+    <x:t>chak.au@parl.gc.ca</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Auguste, Tatiana</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ourcommons.ca/Members/en/tatiana-auguste(122753)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Terrebonne</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ourcommons.ca/Members/en/constituencies/terrebonne(1047)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Quebec</x:t>
+  </x:si>
+  <x:si>
+    <x:t>tatiana.auguste@parl.gc.ca</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Baber, Roman</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ourcommons.ca/Members/en/roman-baber(123276)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>York Centre</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ourcommons.ca/Members/en/constituencies/york-centre(1172)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>416-638-9030</x:t>
   </x:si>
   <x:si>
     <x:t>British Columbia</x:t>
   </x:si>
   <x:si>
-    <x:t>1-800-665-8711</x:t>
-  </x:si>
-  <x:si>
-    <x:t>dan.albas@parl.gc.ca</x:t>
+    <x:t>roman.baber@parl.gc.ca</x:t>
   </x:si>
   <x:si>
     <x:t>Ali, Hon. Shafqat</x:t>
@@ -251,6 +248,9 @@
   </x:si>
   <x:si>
     <x:t>scott.anderson@parl.gc.ca</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Anstey, Carol</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -635,288 +635,288 @@
     </x:row>
     <x:row r="2" spans="1:8">
       <x:c r="A2" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
         <x:v>8</x:v>
-      </x:c>
-      <x:c r="B2" s="0" t="s">
-        <x:v>9</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="E2" s="0" t="s">
+      <x:c r="F2" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="F2" s="0" t="s">
+      <x:c r="G2" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="G2" s="0" t="s">
+      <x:c r="H2" s="0" t="s">
         <x:v>14</x:v>
-      </x:c>
-      <x:c r="H2" s="0" t="s">
-        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
       <x:c r="A3" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="B3" s="0" t="s">
+      <x:c r="C3" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="s">
+      <x:c r="E3" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="E3" s="0" t="s">
+      <x:c r="F3" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="G3" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="F3" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="G3" s="0" t="s">
+      <x:c r="H3" s="0" t="s">
         <x:v>22</x:v>
-      </x:c>
-      <x:c r="H3" s="0" t="s">
-        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:8">
       <x:c r="A4" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
         <x:v>24</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>25</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="E4" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
       <x:c r="F4" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="G4" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="H4" s="0" t="s">
         <x:v>28</x:v>
-      </x:c>
-      <x:c r="H4" s="0" t="s">
-        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:8">
       <x:c r="A5" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
         <x:v>30</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>31</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
         <x:v>32</x:v>
       </x:c>
-      <x:c r="E5" s="0" t="s">
+      <x:c r="F5" s="0" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="F5" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
       <x:c r="G5" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="H5" s="0" t="s">
         <x:v>34</x:v>
-      </x:c>
-      <x:c r="H5" s="0" t="s">
-        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
       <x:c r="A6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
         <x:v>36</x:v>
-      </x:c>
-      <x:c r="B6" s="0" t="s">
-        <x:v>37</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E6" s="0" t="s">
+      <x:c r="F6" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="G6" s="0" t="s">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="F6" s="0" t="s">
-        <x:v>40</x:v>
-      </x:c>
-      <x:c r="G6" s="0" t="s">
+      <x:c r="H6" s="0" t="s">
         <x:v>41</x:v>
-      </x:c>
-      <x:c r="H6" s="0" t="s">
-        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:8">
       <x:c r="A7" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
         <x:v>43</x:v>
-      </x:c>
-      <x:c r="B7" s="0" t="s">
-        <x:v>44</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
         <x:v>45</x:v>
-      </x:c>
-      <x:c r="E7" s="0" t="s">
-        <x:v>46</x:v>
       </x:c>
       <x:c r="F7" s="0" t="s">
         <x:v>21</x:v>
       </x:c>
       <x:c r="G7" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="H7" s="0" t="s">
         <x:v>47</x:v>
-      </x:c>
-      <x:c r="H7" s="0" t="s">
-        <x:v>48</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:8">
       <x:c r="A8" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
         <x:v>49</x:v>
-      </x:c>
-      <x:c r="B8" s="0" t="s">
-        <x:v>50</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
         <x:v>51</x:v>
-      </x:c>
-      <x:c r="E8" s="0" t="s">
-        <x:v>52</x:v>
       </x:c>
       <x:c r="F8" s="0" t="s">
         <x:v>21</x:v>
       </x:c>
       <x:c r="G8" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="H8" s="0" t="s">
         <x:v>53</x:v>
-      </x:c>
-      <x:c r="H8" s="0" t="s">
-        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:8">
       <x:c r="A9" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
         <x:v>55</x:v>
-      </x:c>
-      <x:c r="B9" s="0" t="s">
-        <x:v>56</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
         <x:v>57</x:v>
       </x:c>
-      <x:c r="E9" s="0" t="s">
+      <x:c r="F9" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="G9" s="0" t="s">
         <x:v>58</x:v>
       </x:c>
-      <x:c r="F9" s="0" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="G9" s="0" t="s">
+      <x:c r="H9" s="0" t="s">
         <x:v>59</x:v>
-      </x:c>
-      <x:c r="H9" s="0" t="s">
-        <x:v>60</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:8">
       <x:c r="A10" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
         <x:v>61</x:v>
-      </x:c>
-      <x:c r="B10" s="0" t="s">
-        <x:v>62</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
         <x:v>63</x:v>
-      </x:c>
-      <x:c r="E10" s="0" t="s">
-        <x:v>64</x:v>
       </x:c>
       <x:c r="F10" s="0" t="s">
         <x:v>21</x:v>
       </x:c>
       <x:c r="G10" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="H10" s="0" t="s">
         <x:v>65</x:v>
-      </x:c>
-      <x:c r="H10" s="0" t="s">
-        <x:v>66</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
       <x:c r="A11" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
         <x:v>67</x:v>
-      </x:c>
-      <x:c r="B11" s="0" t="s">
-        <x:v>68</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="s">
         <x:v>69</x:v>
-      </x:c>
-      <x:c r="E11" s="0" t="s">
-        <x:v>70</x:v>
       </x:c>
       <x:c r="F11" s="0" t="s">
         <x:v>21</x:v>
       </x:c>
       <x:c r="G11" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="H11" s="0" t="s">
         <x:v>71</x:v>
-      </x:c>
-      <x:c r="H11" s="0" t="s">
-        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
       <x:c r="A12" s="0" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
         <x:v>73</x:v>
-      </x:c>
-      <x:c r="B12" s="0" t="s">
-        <x:v>74</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="E12" s="0" t="s">
         <x:v>75</x:v>
-      </x:c>
-      <x:c r="E12" s="0" t="s">
-        <x:v>76</x:v>
       </x:c>
       <x:c r="F12" s="0" t="s">
         <x:v>40</x:v>
       </x:c>
       <x:c r="G12" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="H12" s="0" t="s">
         <x:v>77</x:v>
-      </x:c>
-      <x:c r="H12" s="0" t="s">
-        <x:v>78</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
testOn variable set with default value instead
</commit_message>
<xml_diff>
--- a/Test Parliament.xlsx
+++ b/Test Parliament.xlsx
@@ -40,15 +40,18 @@
     <x:t>Email</x:t>
   </x:si>
   <x:si>
+    <x:t>Anstey, Carol</x:t>
+  </x:si>
+  <x:si>
     <x:t>https://www.ourcommons.ca/Members/en/carol-anstey(109872)</x:t>
   </x:si>
   <x:si>
+    <x:t>Conservative</x:t>
+  </x:si>
+  <x:si>
     <x:t>Long Range Mountains</x:t>
   </x:si>
   <x:si>
-    <x:t>Conservative</x:t>
-  </x:si>
-  <x:si>
     <x:t>https://www.ourcommons.ca/Members/en/constituencies/long-range-mountains(947)</x:t>
   </x:si>
   <x:si>
@@ -70,75 +73,78 @@
     <x:t>Kamloops—Shuswap—Central Rockies</x:t>
   </x:si>
   <x:si>
+    <x:t>https://www.ourcommons.ca/Members/en/constituencies/kamloops-shuswap-central-rockies(1253)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>British Columbia</x:t>
+  </x:si>
+  <x:si>
+    <x:t>778-283-9700</x:t>
+  </x:si>
+  <x:si>
+    <x:t>mel.arnold@parl.gc.ca</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Au, Chak</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ourcommons.ca/Members/en/chak-au(123608)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Richmond Centre—Marpole</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ourcommons.ca/Members/en/constituencies/richmond-centre-marpole(1266)</x:t>
+  </x:si>
+  <x:si>
+    <x:t/>
+  </x:si>
+  <x:si>
+    <x:t>chak.au@parl.gc.ca</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Auguste, Tatiana</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ourcommons.ca/Members/en/tatiana-auguste(122753)</x:t>
+  </x:si>
+  <x:si>
     <x:t>Liberal</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.ourcommons.ca/Members/en/constituencies/kamloops-shuswap-central-rockies(1253)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>778-283-9700</x:t>
+    <x:t>Terrebonne</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ourcommons.ca/Members/en/constituencies/terrebonne(1047)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Quebec</x:t>
+  </x:si>
+  <x:si>
+    <x:t>450-964-4919</x:t>
+  </x:si>
+  <x:si>
+    <x:t>tatiana.auguste@parl.gc.ca</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Baber, Roman</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ourcommons.ca/Members/en/roman-baber(123276)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>York Centre</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ourcommons.ca/Members/en/constituencies/york-centre(1172)</x:t>
   </x:si>
   <x:si>
     <x:t>Ontario</x:t>
   </x:si>
   <x:si>
-    <x:t>mel.arnold@parl.gc.ca</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Au, Chak</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ourcommons.ca/Members/en/chak-au(123608)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Richmond Centre—Marpole</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ourcommons.ca/Members/en/constituencies/richmond-centre-marpole(1266)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>450-964-4919</x:t>
-  </x:si>
-  <x:si>
-    <x:t>chak.au@parl.gc.ca</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Auguste, Tatiana</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ourcommons.ca/Members/en/tatiana-auguste(122753)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Terrebonne</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ourcommons.ca/Members/en/constituencies/terrebonne(1047)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Quebec</x:t>
-  </x:si>
-  <x:si>
-    <x:t>tatiana.auguste@parl.gc.ca</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Baber, Roman</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ourcommons.ca/Members/en/roman-baber(123276)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>York Centre</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ourcommons.ca/Members/en/constituencies/york-centre(1172)</x:t>
-  </x:si>
-  <x:si>
     <x:t>416-638-9030</x:t>
   </x:si>
   <x:si>
-    <x:t>British Columbia</x:t>
-  </x:si>
-  <x:si>
     <x:t>roman.baber@parl.gc.ca</x:t>
   </x:si>
   <x:si>
@@ -244,13 +250,7 @@
     <x:t>https://www.ourcommons.ca/Members/en/constituencies/vernon-lake-country-monashee(1280)</x:t>
   </x:si>
   <x:si>
-    <x:t/>
-  </x:si>
-  <x:si>
     <x:t>scott.anderson@parl.gc.ca</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Anstey, Carol</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -635,51 +635,51 @@
     </x:row>
     <x:row r="2" spans="1:8">
       <x:c r="A2" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="F2" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="G2" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="H2" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
       <x:c r="A3" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E3" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
       <x:c r="F3" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="G3" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="H3" s="0" t="s">
         <x:v>22</x:v>
@@ -702,10 +702,10 @@
         <x:v>26</x:v>
       </x:c>
       <x:c r="F4" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="G4" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="H4" s="0" t="s">
         <x:v>28</x:v>
@@ -719,204 +719,204 @@
         <x:v>30</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="F5" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="G5" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="H5" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
       <x:c r="A6" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="F6" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="G6" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H6" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:8">
       <x:c r="A7" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="E7" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="F7" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="G7" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="H7" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>49</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:8">
       <x:c r="A8" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="E8" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="F8" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="G8" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="H8" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:8">
       <x:c r="A9" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="E9" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="F9" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="G9" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="H9" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:8">
       <x:c r="A10" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="E10" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="F10" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="G10" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="H10" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
       <x:c r="A11" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="E11" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="F11" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="G11" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="H11" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
       <x:c r="A12" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="E12" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="F12" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="G12" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="H12" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
fewer testing rows for a faster video
</commit_message>
<xml_diff>
--- a/Test Parliament.xlsx
+++ b/Test Parliament.xlsx
@@ -40,28 +40,7 @@
     <x:t>Email</x:t>
   </x:si>
   <x:si>
-    <x:t>Anstey, Carol</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ourcommons.ca/Members/en/carol-anstey(109872)</x:t>
-  </x:si>
-  <x:si>
     <x:t>Conservative</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Long Range Mountains</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ourcommons.ca/Members/en/constituencies/long-range-mountains(947)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Newfoundland and Labrador</x:t>
-  </x:si>
-  <x:si>
-    <x:t>709-637-4655</x:t>
-  </x:si>
-  <x:si>
-    <x:t>carol.anstey@parl.gc.ca</x:t>
   </x:si>
   <x:si>
     <x:t>Arnold, Mel</x:t>
@@ -635,13 +614,13 @@
     </x:row>
     <x:row r="2" spans="1:8">
       <x:c r="A2" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
         <x:v>8</x:v>
-      </x:c>
-      <x:c r="B2" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>10</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
         <x:v>11</x:v>
@@ -667,7 +646,7 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
         <x:v>18</x:v>
@@ -676,24 +655,24 @@
         <x:v>19</x:v>
       </x:c>
       <x:c r="F3" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="G3" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="G3" s="0" t="s">
+      <x:c r="H3" s="0" t="s">
         <x:v>21</x:v>
-      </x:c>
-      <x:c r="H3" s="0" t="s">
-        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:8">
       <x:c r="A4" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="B4" s="0" t="s">
+      <x:c r="C4" s="0" t="s">
         <x:v>24</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>10</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
         <x:v>25</x:v>
@@ -702,221 +681,221 @@
         <x:v>26</x:v>
       </x:c>
       <x:c r="F4" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="G4" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="H4" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:8">
       <x:c r="A5" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="G5" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="H5" s="0" t="s">
         <x:v>29</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="C5" s="0" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="D5" s="0" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="E5" s="0" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="F5" s="0" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="G5" s="0" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="H5" s="0" t="s">
-        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
       <x:c r="A6" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="F6" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="G6" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="H6" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:8">
       <x:c r="A7" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="E7" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="F7" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="G7" s="0" t="s">
         <x:v>41</x:v>
       </x:c>
-      <x:c r="G7" s="0" t="s">
-        <x:v>48</x:v>
-      </x:c>
       <x:c r="H7" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:8">
       <x:c r="A8" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="E8" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="F8" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="G8" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="H8" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>48</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:8">
       <x:c r="A9" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="E9" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="F9" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="G9" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H9" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:8">
       <x:c r="A10" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="E10" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="F10" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="G10" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="H10" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>60</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8">
       <x:c r="A11" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="E11" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="F11" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="G11" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="H11" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>66</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8">
       <x:c r="A12" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="E12" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="F12" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="G12" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="G12" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
       <x:c r="H12" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>71</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
edited Excel of all members to remove Mark Carney and create 1 giant list I can email
</commit_message>
<xml_diff>
--- a/Test Parliament.xlsx
+++ b/Test Parliament.xlsx
@@ -40,13 +40,13 @@
     <x:t>Email</x:t>
   </x:si>
   <x:si>
+    <x:t>Arnold, Mel</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ourcommons.ca/Members/en/mel-arnold(89294)</x:t>
+  </x:si>
+  <x:si>
     <x:t>Conservative</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Arnold, Mel</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ourcommons.ca/Members/en/mel-arnold(89294)</x:t>
   </x:si>
   <x:si>
     <x:t>Kamloops—Shuswap—Central Rockies</x:t>
@@ -614,13 +614,13 @@
     </x:row>
     <x:row r="2" spans="1:8">
       <x:c r="A2" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="B2" s="0" t="s">
+      <x:c r="C2" s="0" t="s">
         <x:v>10</x:v>
-      </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>8</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
         <x:v>11</x:v>
@@ -646,7 +646,7 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
         <x:v>18</x:v>
@@ -724,7 +724,7 @@
         <x:v>31</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
         <x:v>32</x:v>
@@ -776,7 +776,7 @@
         <x:v>44</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
         <x:v>45</x:v>
@@ -880,7 +880,7 @@
         <x:v>68</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
         <x:v>69</x:v>

</xml_diff>